<commit_message>
1. Created function to process institute name into machine spreadsheet
</commit_message>
<xml_diff>
--- a/lib/machines/templates/machines.xlsx
+++ b/lib/machines/templates/machines.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="266">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machines</t>
   </si>
@@ -91,7 +91,29 @@
     <t xml:space="preserve">Internal notes</t>
   </si>
   <si>
-    <t xml:space="preserve">CMIP6 Institute Machine</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="18"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Example Machine </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="18"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(note example institute is NERC but the inputs are not official)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Properties of a computer/system/platform/machine which is used to run CMIP6 simulations.</t>
@@ -836,6 +858,9 @@
     <t xml:space="preserve">LIG127k</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;institute name will be processed here&gt; Machine for CMIP6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Did this machine run each of the following models? For each model, if it was run on this machine select YES, else select NO.
 Note that the listing below should cover all of the models that your institute will be running for CMIP6 (on one of your machines, but perhaps not this one) and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this.</t>
   </si>
@@ -889,7 +914,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -939,13 +964,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <color rgb="FFCE181E"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
@@ -967,6 +985,15 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
@@ -1085,14 +1112,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FFED1C24"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="14"/>
       <color rgb="FFED1C24"/>
       <name val="Helvetica Neue"/>
@@ -1129,7 +1148,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1140,12 +1159,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94070A"/>
-        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1254,7 +1267,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1295,15 +1308,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1319,11 +1332,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1351,11 +1364,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1367,7 +1380,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1387,7 +1400,7 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1411,63 +1424,63 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1483,7 +1496,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1496,10 +1509,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1559,7 +1568,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1567,15 +1580,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1602,7 +1611,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF94070A"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -1662,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1779,7 +1788,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12386,8 +12395,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B437" activeCellId="0" sqref="B437"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12406,17 +12415,17 @@
       <c r="A1" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="0"/>
@@ -12434,11 +12443,11 @@
     </row>
     <row r="4" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="0"/>
       <c r="F4" s="12"/>
     </row>
@@ -12464,7 +12473,7 @@
     </row>
     <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="0"/>
@@ -12493,13 +12502,13 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="66"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
       <c r="F10" s="12"/>
@@ -12536,39 +12545,39 @@
       <c r="A14" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="66"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
       <c r="F14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="60"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="60"/>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="66"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
       <c r="E17" s="0"/>
       <c r="F17" s="29"/>
     </row>
@@ -12602,7 +12611,7 @@
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="61" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="0"/>
@@ -12612,7 +12621,7 @@
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
-      <c r="B22" s="62"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="0"/>
       <c r="D22" s="23"/>
       <c r="E22" s="0"/>
@@ -12631,32 +12640,32 @@
       <c r="F23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="66"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
       <c r="F24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="65"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
       <c r="F25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="65"/>
-      <c r="B26" s="67" t="s">
+      <c r="A26" s="64"/>
+      <c r="B26" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
       <c r="E26" s="0"/>
       <c r="F26" s="29"/>
     </row>
@@ -12689,13 +12698,13 @@
       <c r="F29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="66"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="0"/>
       <c r="E30" s="0"/>
       <c r="F30" s="0"/>
@@ -12732,28 +12741,28 @@
       <c r="A34" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="66"/>
+      <c r="C34" s="65"/>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="68"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="66"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
       <c r="D35" s="0"/>
       <c r="E35" s="0"/>
       <c r="F35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="69"/>
-      <c r="B36" s="66" t="s">
+      <c r="A36" s="68"/>
+      <c r="B36" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="66"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
@@ -12790,34 +12799,34 @@
       <c r="A40" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="66"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="0"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="69"/>
-      <c r="B41" s="66"/>
-      <c r="C41" s="66"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="0"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="69"/>
-      <c r="B42" s="66" t="s">
+      <c r="A42" s="68"/>
+      <c r="B42" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="66"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="0"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="70" t="s">
+      <c r="A43" s="69" t="s">
         <v>45</v>
       </c>
       <c r="B43" s="33"/>
@@ -12827,15 +12836,15 @@
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="0"/>
       <c r="F44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="70" t="s">
+      <c r="A45" s="69" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="33"/>
@@ -12865,13 +12874,13 @@
       <c r="F47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="66"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="0"/>
       <c r="E48" s="0"/>
       <c r="F48" s="0"/>
@@ -12906,7 +12915,7 @@
     </row>
     <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
-      <c r="B52" s="62" t="s">
+      <c r="B52" s="61" t="s">
         <v>53</v>
       </c>
       <c r="C52" s="0"/>
@@ -12935,32 +12944,32 @@
       <c r="F54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B55" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="66"/>
+      <c r="C55" s="65"/>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="65"/>
-      <c r="B56" s="66"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="62"/>
+      <c r="A56" s="64"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="61"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="65"/>
-      <c r="B57" s="67" t="s">
+      <c r="A57" s="64"/>
+      <c r="B57" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="67"/>
-      <c r="D57" s="67"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
     </row>
@@ -12993,13 +13002,13 @@
       <c r="F60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B61" s="66" t="s">
+      <c r="B61" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="66"/>
+      <c r="C61" s="65"/>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
@@ -13034,7 +13043,7 @@
     </row>
     <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
-      <c r="B65" s="62" t="s">
+      <c r="B65" s="61" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="0"/>
@@ -13044,19 +13053,19 @@
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
+      <c r="B66" s="63"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
       <c r="E66" s="0"/>
       <c r="F66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="65.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
       <c r="E67" s="0"/>
       <c r="F67" s="0"/>
     </row>
@@ -13082,18 +13091,18 @@
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="60"/>
-      <c r="B70" s="62" t="s">
+      <c r="B70" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="66"/>
+      <c r="C70" s="65"/>
       <c r="D70" s="0"/>
       <c r="E70" s="0"/>
       <c r="F70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="65"/>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
+      <c r="A71" s="64"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="65"/>
       <c r="D71" s="0"/>
       <c r="E71" s="0"/>
       <c r="F71" s="0"/>
@@ -13111,13 +13120,13 @@
       <c r="F72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="66" t="s">
+      <c r="B73" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C73" s="66"/>
+      <c r="C73" s="65"/>
       <c r="D73" s="0"/>
       <c r="E73" s="0"/>
       <c r="F73" s="0"/>
@@ -13151,13 +13160,13 @@
       <c r="F76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="65" t="s">
+      <c r="A77" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B77" s="66" t="s">
+      <c r="B77" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="66"/>
+      <c r="C77" s="65"/>
       <c r="D77" s="0"/>
       <c r="E77" s="0"/>
       <c r="F77" s="0"/>
@@ -13191,32 +13200,32 @@
       <c r="F80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="65" t="s">
+      <c r="A81" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B81" s="66" t="s">
+      <c r="B81" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C81" s="66"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
       <c r="F81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="65"/>
-      <c r="B82" s="66"/>
-      <c r="C82" s="66"/>
+      <c r="A82" s="64"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="0"/>
       <c r="E82" s="0"/>
       <c r="F82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="65"/>
-      <c r="B83" s="67" t="s">
+      <c r="A83" s="64"/>
+      <c r="B83" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C83" s="67"/>
-      <c r="D83" s="67"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="66"/>
       <c r="E83" s="0"/>
       <c r="F83" s="0"/>
     </row>
@@ -13249,13 +13258,13 @@
       <c r="F86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="65" t="s">
+      <c r="A87" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="66" t="s">
+      <c r="B87" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="66"/>
+      <c r="C87" s="65"/>
       <c r="D87" s="0"/>
       <c r="E87" s="0"/>
       <c r="F87" s="0"/>
@@ -13289,13 +13298,13 @@
       <c r="F90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="65" t="s">
+      <c r="A91" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B91" s="66" t="s">
+      <c r="B91" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C91" s="66"/>
+      <c r="C91" s="65"/>
       <c r="D91" s="0"/>
       <c r="E91" s="0"/>
       <c r="F91" s="0"/>
@@ -13332,10 +13341,10 @@
       <c r="A95" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="B95" s="66" t="s">
+      <c r="B95" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="C95" s="66"/>
+      <c r="C95" s="65"/>
       <c r="D95" s="0"/>
       <c r="E95" s="0"/>
       <c r="F95" s="29"/>
@@ -13369,13 +13378,13 @@
       <c r="F98" s="29"/>
     </row>
     <row r="99" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="65" t="s">
+      <c r="A99" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B99" s="66" t="s">
+      <c r="B99" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="C99" s="66"/>
+      <c r="C99" s="65"/>
       <c r="D99" s="0"/>
       <c r="E99" s="0"/>
       <c r="F99" s="29"/>
@@ -13913,13 +13922,13 @@
       <c r="F152" s="29"/>
     </row>
     <row r="153" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="65" t="s">
+      <c r="A153" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B153" s="66" t="s">
+      <c r="B153" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C153" s="66"/>
+      <c r="C153" s="65"/>
       <c r="D153" s="0"/>
       <c r="E153" s="0"/>
       <c r="F153" s="29"/>
@@ -13953,13 +13962,13 @@
       <c r="F156" s="29"/>
     </row>
     <row r="157" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="65" t="s">
+      <c r="A157" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B157" s="66" t="s">
+      <c r="B157" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="C157" s="66"/>
+      <c r="C157" s="65"/>
       <c r="D157" s="0"/>
       <c r="E157" s="0"/>
       <c r="F157" s="29"/>
@@ -13993,13 +14002,13 @@
       <c r="F160" s="29"/>
     </row>
     <row r="161" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="65" t="s">
+      <c r="A161" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B161" s="66" t="s">
+      <c r="B161" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="C161" s="66"/>
+      <c r="C161" s="65"/>
       <c r="D161" s="0"/>
       <c r="E161" s="0"/>
       <c r="F161" s="29"/>
@@ -14036,10 +14045,10 @@
       <c r="A165" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B165" s="66" t="s">
+      <c r="B165" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="C165" s="66"/>
+      <c r="C165" s="65"/>
       <c r="D165" s="0"/>
       <c r="E165" s="0"/>
       <c r="F165" s="29"/>
@@ -14073,13 +14082,13 @@
       <c r="F168" s="29"/>
     </row>
     <row r="169" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="65" t="s">
+      <c r="A169" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B169" s="66" t="s">
+      <c r="B169" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="C169" s="66"/>
+      <c r="C169" s="65"/>
       <c r="D169" s="0"/>
       <c r="E169" s="0"/>
       <c r="F169" s="29"/>
@@ -14114,18 +14123,18 @@
     </row>
     <row r="173" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="60"/>
-      <c r="B173" s="62" t="s">
+      <c r="B173" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C173" s="66"/>
+      <c r="C173" s="65"/>
       <c r="D173" s="0"/>
       <c r="E173" s="0"/>
       <c r="F173" s="29"/>
     </row>
     <row r="174" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="65"/>
-      <c r="B174" s="66"/>
-      <c r="C174" s="66"/>
+      <c r="A174" s="64"/>
+      <c r="B174" s="65"/>
+      <c r="C174" s="65"/>
       <c r="D174" s="0"/>
       <c r="E174" s="0"/>
       <c r="F174" s="29"/>
@@ -14143,13 +14152,13 @@
       <c r="F175" s="29"/>
     </row>
     <row r="176" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="65" t="s">
+      <c r="A176" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B176" s="66" t="s">
+      <c r="B176" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C176" s="66"/>
+      <c r="C176" s="65"/>
       <c r="D176" s="0"/>
       <c r="E176" s="0"/>
       <c r="F176" s="29"/>
@@ -14183,13 +14192,13 @@
       <c r="F179" s="29"/>
     </row>
     <row r="180" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="65" t="s">
+      <c r="A180" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B180" s="66" t="s">
+      <c r="B180" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="C180" s="66"/>
+      <c r="C180" s="65"/>
       <c r="D180" s="0"/>
       <c r="E180" s="0"/>
       <c r="F180" s="29"/>
@@ -14223,32 +14232,32 @@
       <c r="F183" s="29"/>
     </row>
     <row r="184" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="65" t="s">
+      <c r="A184" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B184" s="66" t="s">
+      <c r="B184" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C184" s="66"/>
+      <c r="C184" s="65"/>
       <c r="D184" s="0"/>
       <c r="E184" s="0"/>
       <c r="F184" s="29"/>
     </row>
     <row r="185" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="65"/>
-      <c r="B185" s="66"/>
-      <c r="C185" s="66"/>
+      <c r="A185" s="64"/>
+      <c r="B185" s="65"/>
+      <c r="C185" s="65"/>
       <c r="D185" s="0"/>
       <c r="E185" s="0"/>
       <c r="F185" s="29"/>
     </row>
     <row r="186" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="65"/>
-      <c r="B186" s="67" t="s">
+      <c r="A186" s="64"/>
+      <c r="B186" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C186" s="67"/>
-      <c r="D186" s="67"/>
+      <c r="C186" s="66"/>
+      <c r="D186" s="66"/>
       <c r="E186" s="0"/>
       <c r="F186" s="29"/>
     </row>
@@ -14281,13 +14290,13 @@
       <c r="F189" s="29"/>
     </row>
     <row r="190" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="65" t="s">
+      <c r="A190" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B190" s="66" t="s">
+      <c r="B190" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="C190" s="66"/>
+      <c r="C190" s="65"/>
       <c r="D190" s="0"/>
       <c r="E190" s="0"/>
       <c r="F190" s="29"/>
@@ -14321,13 +14330,13 @@
       <c r="F193" s="29"/>
     </row>
     <row r="194" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="65" t="s">
+      <c r="A194" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B194" s="66" t="s">
+      <c r="B194" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C194" s="66"/>
+      <c r="C194" s="65"/>
       <c r="D194" s="0"/>
       <c r="E194" s="0"/>
       <c r="F194" s="29"/>
@@ -14364,10 +14373,10 @@
       <c r="A198" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="B198" s="66" t="s">
+      <c r="B198" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="C198" s="66"/>
+      <c r="C198" s="65"/>
       <c r="D198" s="0"/>
       <c r="E198" s="0"/>
       <c r="F198" s="29"/>
@@ -14401,13 +14410,13 @@
       <c r="F201" s="29"/>
     </row>
     <row r="202" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="65" t="s">
+      <c r="A202" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B202" s="66" t="s">
+      <c r="B202" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="C202" s="66"/>
+      <c r="C202" s="65"/>
       <c r="D202" s="0"/>
       <c r="E202" s="0"/>
       <c r="F202" s="29"/>
@@ -14945,13 +14954,13 @@
       <c r="F255" s="29"/>
     </row>
     <row r="256" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="65" t="s">
+      <c r="A256" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B256" s="66" t="s">
+      <c r="B256" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C256" s="66"/>
+      <c r="C256" s="65"/>
       <c r="D256" s="0"/>
       <c r="E256" s="0"/>
       <c r="F256" s="29"/>
@@ -14985,13 +14994,13 @@
       <c r="F259" s="29"/>
     </row>
     <row r="260" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="65" t="s">
+      <c r="A260" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B260" s="66" t="s">
+      <c r="B260" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="C260" s="66"/>
+      <c r="C260" s="65"/>
       <c r="D260" s="0"/>
       <c r="E260" s="0"/>
       <c r="F260" s="29"/>
@@ -15025,13 +15034,13 @@
       <c r="F263" s="29"/>
     </row>
     <row r="264" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="65" t="s">
+      <c r="A264" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B264" s="66" t="s">
+      <c r="B264" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="C264" s="66"/>
+      <c r="C264" s="65"/>
       <c r="D264" s="0"/>
       <c r="E264" s="0"/>
       <c r="F264" s="29"/>
@@ -15065,13 +15074,13 @@
       <c r="F267" s="29"/>
     </row>
     <row r="268" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="65" t="s">
+      <c r="A268" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="B268" s="66" t="s">
+      <c r="B268" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="C268" s="66"/>
+      <c r="C268" s="65"/>
       <c r="D268" s="0"/>
       <c r="E268" s="0"/>
       <c r="F268" s="29"/>
@@ -15105,13 +15114,13 @@
       <c r="F271" s="29"/>
     </row>
     <row r="272" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="65" t="s">
+      <c r="A272" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B272" s="66" t="s">
+      <c r="B272" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="C272" s="66"/>
+      <c r="C272" s="65"/>
       <c r="D272" s="0"/>
       <c r="E272" s="0"/>
       <c r="F272" s="29"/>
@@ -15145,7 +15154,7 @@
     </row>
     <row r="276" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0"/>
-      <c r="B276" s="62" t="s">
+      <c r="B276" s="61" t="s">
         <v>162</v>
       </c>
       <c r="C276" s="0"/>
@@ -15156,18 +15165,18 @@
     <row r="277" customFormat="false" ht="22.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="0"/>
       <c r="B277" s="0"/>
-      <c r="C277" s="64"/>
-      <c r="D277" s="64"/>
+      <c r="C277" s="63"/>
+      <c r="D277" s="63"/>
       <c r="E277" s="0"/>
       <c r="F277" s="29"/>
     </row>
     <row r="278" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="0"/>
-      <c r="B278" s="72" t="s">
+      <c r="B278" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="C278" s="72"/>
-      <c r="D278" s="72"/>
+      <c r="C278" s="71"/>
+      <c r="D278" s="71"/>
       <c r="E278" s="0"/>
       <c r="F278" s="29"/>
     </row>
@@ -15193,18 +15202,18 @@
     </row>
     <row r="281" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="60"/>
-      <c r="B281" s="62" t="s">
+      <c r="B281" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="C281" s="66"/>
+      <c r="C281" s="65"/>
       <c r="D281" s="0"/>
       <c r="E281" s="0"/>
       <c r="F281" s="29"/>
     </row>
     <row r="282" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="65"/>
-      <c r="B282" s="66"/>
-      <c r="C282" s="66"/>
+      <c r="A282" s="64"/>
+      <c r="B282" s="65"/>
+      <c r="C282" s="65"/>
       <c r="D282" s="0"/>
       <c r="E282" s="0"/>
       <c r="F282" s="29"/>
@@ -15222,13 +15231,13 @@
       <c r="F283" s="29"/>
     </row>
     <row r="284" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="65" t="s">
+      <c r="A284" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B284" s="66" t="s">
+      <c r="B284" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="C284" s="66"/>
+      <c r="C284" s="65"/>
       <c r="D284" s="0"/>
       <c r="E284" s="0"/>
       <c r="F284" s="29"/>
@@ -15265,28 +15274,28 @@
       <c r="A288" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="B288" s="66" t="s">
+      <c r="B288" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="C288" s="66"/>
+      <c r="C288" s="65"/>
       <c r="D288" s="0"/>
       <c r="E288" s="0"/>
       <c r="F288" s="29"/>
     </row>
     <row r="289" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="69"/>
-      <c r="B289" s="66"/>
-      <c r="C289" s="66"/>
+      <c r="A289" s="68"/>
+      <c r="B289" s="65"/>
+      <c r="C289" s="65"/>
       <c r="D289" s="0"/>
       <c r="E289" s="0"/>
       <c r="F289" s="29"/>
     </row>
     <row r="290" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="69"/>
-      <c r="B290" s="66" t="s">
+      <c r="A290" s="68"/>
+      <c r="B290" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C290" s="66"/>
+      <c r="C290" s="65"/>
       <c r="D290" s="0"/>
       <c r="E290" s="0"/>
       <c r="F290" s="29"/>
@@ -15336,13 +15345,13 @@
       <c r="F295" s="29"/>
     </row>
     <row r="296" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="65" t="s">
+      <c r="A296" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B296" s="66" t="s">
+      <c r="B296" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="C296" s="66"/>
+      <c r="C296" s="65"/>
       <c r="D296" s="0"/>
       <c r="E296" s="0"/>
       <c r="F296" s="29"/>
@@ -15377,26 +15386,26 @@
       <c r="A300" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B300" s="66" t="s">
+      <c r="B300" s="65" t="s">
         <v>180</v>
       </c>
-      <c r="C300" s="66"/>
+      <c r="C300" s="65"/>
       <c r="D300" s="0"/>
       <c r="E300" s="0"/>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="60"/>
-      <c r="B301" s="66"/>
-      <c r="C301" s="66"/>
+      <c r="B301" s="65"/>
+      <c r="C301" s="65"/>
       <c r="D301" s="0"/>
       <c r="E301" s="0"/>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="60"/>
-      <c r="B302" s="66" t="s">
+      <c r="B302" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="C302" s="66"/>
+      <c r="C302" s="65"/>
       <c r="D302" s="0"/>
       <c r="E302" s="0"/>
     </row>
@@ -15426,29 +15435,29 @@
       <c r="E305" s="0"/>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="65" t="s">
+      <c r="A306" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B306" s="66" t="s">
+      <c r="B306" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="C306" s="66"/>
+      <c r="C306" s="65"/>
       <c r="D306" s="0"/>
       <c r="E306" s="0"/>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="65"/>
-      <c r="B307" s="66"/>
-      <c r="C307" s="66"/>
+      <c r="A307" s="64"/>
+      <c r="B307" s="65"/>
+      <c r="C307" s="65"/>
       <c r="D307" s="0"/>
       <c r="E307" s="0"/>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="65"/>
-      <c r="B308" s="66" t="s">
+      <c r="A308" s="64"/>
+      <c r="B308" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C308" s="66"/>
+      <c r="C308" s="65"/>
       <c r="D308" s="0"/>
       <c r="E308" s="0"/>
     </row>
@@ -15479,33 +15488,33 @@
     </row>
     <row r="312" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="60"/>
-      <c r="B312" s="62" t="s">
+      <c r="B312" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="C312" s="66"/>
+      <c r="C312" s="65"/>
       <c r="D312" s="0"/>
       <c r="E312" s="0"/>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="65"/>
-      <c r="B313" s="66"/>
-      <c r="C313" s="66"/>
+      <c r="A313" s="64"/>
+      <c r="B313" s="65"/>
+      <c r="C313" s="65"/>
       <c r="D313" s="0"/>
       <c r="E313" s="0"/>
     </row>
     <row r="314" customFormat="false" ht="29.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A314" s="65"/>
-      <c r="B314" s="73" t="s">
+      <c r="A314" s="64"/>
+      <c r="B314" s="72" t="s">
         <v>188</v>
       </c>
-      <c r="C314" s="73"/>
-      <c r="D314" s="73"/>
+      <c r="C314" s="72"/>
+      <c r="D314" s="72"/>
       <c r="E314" s="0"/>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="65"/>
-      <c r="B315" s="66"/>
-      <c r="C315" s="66"/>
+      <c r="A315" s="64"/>
+      <c r="B315" s="65"/>
+      <c r="C315" s="65"/>
       <c r="D315" s="0"/>
       <c r="E315" s="0"/>
     </row>
@@ -15521,13 +15530,13 @@
       <c r="E316" s="0"/>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="65" t="s">
+      <c r="A317" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B317" s="66" t="s">
+      <c r="B317" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="C317" s="66"/>
+      <c r="C317" s="65"/>
       <c r="D317" s="0"/>
       <c r="E317" s="0"/>
     </row>
@@ -15560,26 +15569,26 @@
       <c r="A321" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="B321" s="66" t="s">
+      <c r="B321" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="C321" s="66"/>
+      <c r="C321" s="65"/>
       <c r="D321" s="0"/>
       <c r="E321" s="0"/>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="69"/>
-      <c r="B322" s="66"/>
-      <c r="C322" s="66"/>
+      <c r="A322" s="68"/>
+      <c r="B322" s="65"/>
+      <c r="C322" s="65"/>
       <c r="D322" s="0"/>
       <c r="E322" s="0"/>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="69"/>
-      <c r="B323" s="66" t="s">
+      <c r="A323" s="68"/>
+      <c r="B323" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C323" s="66"/>
+      <c r="C323" s="65"/>
       <c r="D323" s="0"/>
       <c r="E323" s="0"/>
     </row>
@@ -15609,13 +15618,13 @@
       <c r="E326" s="0"/>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="65" t="s">
+      <c r="A327" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B327" s="66" t="s">
+      <c r="B327" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="C327" s="66"/>
+      <c r="C327" s="65"/>
       <c r="D327" s="0"/>
       <c r="E327" s="0"/>
     </row>
@@ -15648,26 +15657,26 @@
       <c r="A331" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B331" s="66" t="s">
+      <c r="B331" s="65" t="s">
         <v>180</v>
       </c>
-      <c r="C331" s="66"/>
+      <c r="C331" s="65"/>
       <c r="D331" s="0"/>
       <c r="E331" s="0"/>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="60"/>
-      <c r="B332" s="66"/>
-      <c r="C332" s="66"/>
+      <c r="B332" s="65"/>
+      <c r="C332" s="65"/>
       <c r="D332" s="0"/>
       <c r="E332" s="0"/>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="60"/>
-      <c r="B333" s="66" t="s">
+      <c r="B333" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="C333" s="66"/>
+      <c r="C333" s="65"/>
       <c r="D333" s="0"/>
       <c r="E333" s="0"/>
     </row>
@@ -15697,29 +15706,29 @@
       <c r="E336" s="0"/>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="65" t="s">
+      <c r="A337" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B337" s="66" t="s">
+      <c r="B337" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="C337" s="66"/>
+      <c r="C337" s="65"/>
       <c r="D337" s="0"/>
       <c r="E337" s="0"/>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="65"/>
-      <c r="B338" s="66"/>
-      <c r="C338" s="66"/>
+      <c r="A338" s="64"/>
+      <c r="B338" s="65"/>
+      <c r="C338" s="65"/>
       <c r="D338" s="0"/>
       <c r="E338" s="0"/>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="65"/>
-      <c r="B339" s="66" t="s">
+      <c r="A339" s="64"/>
+      <c r="B339" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C339" s="66"/>
+      <c r="C339" s="65"/>
       <c r="D339" s="0"/>
       <c r="E339" s="0"/>
     </row>
@@ -15748,7 +15757,7 @@
     </row>
     <row r="343" customFormat="false" ht="28.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="0"/>
-      <c r="B343" s="62" t="s">
+      <c r="B343" s="61" t="s">
         <v>198</v>
       </c>
       <c r="C343" s="0"/>
@@ -15772,13 +15781,13 @@
       <c r="E345" s="0"/>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="65" t="s">
+      <c r="A346" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B346" s="66" t="s">
+      <c r="B346" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="C346" s="66"/>
+      <c r="C346" s="65"/>
       <c r="D346" s="0"/>
       <c r="E346" s="0"/>
     </row>
@@ -15808,13 +15817,13 @@
       <c r="E349" s="0"/>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="65" t="s">
+      <c r="A350" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B350" s="66" t="s">
+      <c r="B350" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="C350" s="66"/>
+      <c r="C350" s="65"/>
       <c r="D350" s="0"/>
       <c r="E350" s="0"/>
     </row>
@@ -15844,13 +15853,13 @@
       <c r="E353" s="0"/>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="65" t="s">
+      <c r="A354" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B354" s="66" t="s">
+      <c r="B354" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="C354" s="66"/>
+      <c r="C354" s="65"/>
       <c r="D354" s="0"/>
       <c r="E354" s="0"/>
     </row>
@@ -15880,29 +15889,29 @@
       <c r="E357" s="0"/>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="65" t="s">
+      <c r="A358" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B358" s="66" t="s">
+      <c r="B358" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="C358" s="66"/>
+      <c r="C358" s="65"/>
       <c r="D358" s="0"/>
       <c r="E358" s="0"/>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="65"/>
-      <c r="B359" s="66"/>
-      <c r="C359" s="66"/>
+      <c r="A359" s="64"/>
+      <c r="B359" s="65"/>
+      <c r="C359" s="65"/>
       <c r="D359" s="0"/>
       <c r="E359" s="0"/>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="65"/>
-      <c r="B360" s="66" t="s">
+      <c r="A360" s="64"/>
+      <c r="B360" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C360" s="66"/>
+      <c r="C360" s="65"/>
       <c r="D360" s="0"/>
       <c r="E360" s="0"/>
     </row>
@@ -15925,7 +15934,7 @@
     </row>
     <row r="364" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0"/>
-      <c r="B364" s="62" t="s">
+      <c r="B364" s="61" t="s">
         <v>212</v>
       </c>
       <c r="C364" s="0"/>
@@ -15948,13 +15957,13 @@
       <c r="D366" s="25"/>
     </row>
     <row r="367" customFormat="false" ht="21.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A367" s="65" t="s">
+      <c r="A367" s="64" t="s">
         <v>215</v>
       </c>
-      <c r="B367" s="66" t="s">
+      <c r="B367" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="C367" s="66"/>
+      <c r="C367" s="65"/>
       <c r="D367" s="0"/>
     </row>
     <row r="368" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15980,13 +15989,13 @@
       <c r="D370" s="25"/>
     </row>
     <row r="371" customFormat="false" ht="23.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A371" s="65" t="s">
+      <c r="A371" s="64" t="s">
         <v>215</v>
       </c>
-      <c r="B371" s="66" t="s">
+      <c r="B371" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="C371" s="66"/>
+      <c r="C371" s="65"/>
       <c r="D371" s="0"/>
     </row>
     <row r="372" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16008,7 +16017,7 @@
     </row>
     <row r="375" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A375" s="0"/>
-      <c r="B375" s="62" t="s">
+      <c r="B375" s="61" t="s">
         <v>221</v>
       </c>
       <c r="C375" s="0"/>
@@ -16016,17 +16025,17 @@
     </row>
     <row r="376" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A376" s="0"/>
-      <c r="B376" s="62"/>
+      <c r="B376" s="61"/>
       <c r="C376" s="0"/>
       <c r="D376" s="23"/>
     </row>
     <row r="377" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A377" s="65"/>
-      <c r="B377" s="67" t="s">
+      <c r="A377" s="64"/>
+      <c r="B377" s="66" t="s">
         <v>222</v>
       </c>
-      <c r="C377" s="67"/>
-      <c r="D377" s="67"/>
+      <c r="C377" s="66"/>
+      <c r="D377" s="66"/>
     </row>
     <row r="378" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="0"/>
@@ -16045,14 +16054,14 @@
       <c r="D379" s="25"/>
     </row>
     <row r="380" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A380" s="65" t="s">
+      <c r="A380" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="B380" s="67" t="s">
+      <c r="B380" s="66" t="s">
         <v>225</v>
       </c>
-      <c r="C380" s="67"/>
-      <c r="D380" s="67"/>
+      <c r="C380" s="66"/>
+      <c r="D380" s="66"/>
     </row>
     <row r="381" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="59"/>
@@ -16061,23 +16070,23 @@
       <c r="D381" s="33"/>
     </row>
     <row r="382" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A382" s="74"/>
-      <c r="B382" s="75"/>
-      <c r="C382" s="75"/>
-      <c r="D382" s="75"/>
+      <c r="A382" s="73"/>
+      <c r="B382" s="74"/>
+      <c r="C382" s="74"/>
+      <c r="D382" s="74"/>
     </row>
     <row r="383" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A383" s="60"/>
-      <c r="B383" s="73" t="s">
+      <c r="B383" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="C383" s="73"/>
-      <c r="D383" s="73"/>
+      <c r="C383" s="72"/>
+      <c r="D383" s="72"/>
     </row>
     <row r="384" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A384" s="68"/>
-      <c r="B384" s="66"/>
-      <c r="C384" s="66"/>
+      <c r="A384" s="67"/>
+      <c r="B384" s="65"/>
+      <c r="C384" s="65"/>
       <c r="D384" s="0"/>
     </row>
     <row r="385" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16091,36 +16100,36 @@
       <c r="D385" s="57"/>
     </row>
     <row r="386" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A386" s="65"/>
-      <c r="B386" s="62" t="s">
+      <c r="A386" s="64"/>
+      <c r="B386" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="C386" s="66"/>
+      <c r="C386" s="65"/>
       <c r="D386" s="0"/>
     </row>
     <row r="387" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A387" s="65"/>
-      <c r="B387" s="62"/>
-      <c r="C387" s="66"/>
+      <c r="A387" s="64"/>
+      <c r="B387" s="61"/>
+      <c r="C387" s="65"/>
       <c r="D387" s="0"/>
     </row>
     <row r="388" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A388" s="65"/>
-      <c r="B388" s="73" t="s">
-        <v>251</v>
-      </c>
-      <c r="C388" s="73"/>
-      <c r="D388" s="73"/>
+      <c r="A388" s="64"/>
+      <c r="B388" s="72" t="s">
+        <v>252</v>
+      </c>
+      <c r="C388" s="72"/>
+      <c r="D388" s="72"/>
     </row>
     <row r="389" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A389" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="B389" s="76" t="s">
+        <v>253</v>
+      </c>
+      <c r="B389" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="C389" s="76"/>
-      <c r="D389" s="76"/>
+      <c r="C389" s="75"/>
+      <c r="D389" s="75"/>
     </row>
     <row r="390" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A390" s="60" t="s">
@@ -16131,20 +16140,20 @@
       <c r="D390" s="33"/>
     </row>
     <row r="391" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A391" s="69"/>
-      <c r="B391" s="66"/>
-      <c r="C391" s="66"/>
+      <c r="A391" s="68"/>
+      <c r="B391" s="65"/>
+      <c r="C391" s="65"/>
       <c r="D391" s="0"/>
     </row>
     <row r="392" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A392" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="B392" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="B392" s="75" t="s">
         <v>232</v>
       </c>
-      <c r="C392" s="76"/>
-      <c r="D392" s="76"/>
+      <c r="C392" s="75"/>
+      <c r="D392" s="75"/>
     </row>
     <row r="393" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A393" s="60" t="s">
@@ -16156,50 +16165,50 @@
     </row>
     <row r="394" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A394" s="60"/>
-      <c r="B394" s="66"/>
-      <c r="C394" s="66"/>
+      <c r="B394" s="65"/>
+      <c r="C394" s="65"/>
       <c r="D394" s="0"/>
     </row>
     <row r="395" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A395" s="77"/>
-      <c r="B395" s="78"/>
-      <c r="C395" s="78"/>
-      <c r="D395" s="79"/>
+      <c r="A395" s="76"/>
+      <c r="B395" s="77"/>
+      <c r="C395" s="77"/>
+      <c r="D395" s="78"/>
     </row>
     <row r="396" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A396" s="77"/>
-      <c r="B396" s="78"/>
-      <c r="C396" s="78"/>
-      <c r="D396" s="79"/>
+      <c r="A396" s="76"/>
+      <c r="B396" s="77"/>
+      <c r="C396" s="77"/>
+      <c r="D396" s="78"/>
     </row>
     <row r="397" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A397" s="77"/>
-      <c r="B397" s="78"/>
-      <c r="C397" s="78"/>
-      <c r="D397" s="79"/>
+      <c r="A397" s="76"/>
+      <c r="B397" s="77"/>
+      <c r="C397" s="77"/>
+      <c r="D397" s="78"/>
     </row>
     <row r="398" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A398" s="77"/>
-      <c r="B398" s="78"/>
-      <c r="C398" s="78"/>
-      <c r="D398" s="79"/>
+      <c r="A398" s="76"/>
+      <c r="B398" s="77"/>
+      <c r="C398" s="77"/>
+      <c r="D398" s="78"/>
     </row>
     <row r="399" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A399" s="77"/>
-      <c r="B399" s="78"/>
-      <c r="C399" s="78"/>
-      <c r="D399" s="79"/>
+      <c r="A399" s="76"/>
+      <c r="B399" s="77"/>
+      <c r="C399" s="77"/>
+      <c r="D399" s="78"/>
     </row>
     <row r="400" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A400" s="77"/>
-      <c r="B400" s="78"/>
-      <c r="C400" s="78"/>
-      <c r="D400" s="79"/>
+      <c r="A400" s="76"/>
+      <c r="B400" s="77"/>
+      <c r="C400" s="77"/>
+      <c r="D400" s="78"/>
     </row>
     <row r="401" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A401" s="60"/>
-      <c r="B401" s="66"/>
-      <c r="C401" s="66"/>
+      <c r="B401" s="65"/>
+      <c r="C401" s="65"/>
       <c r="D401" s="0"/>
     </row>
     <row r="402" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16221,9 +16230,9 @@
       <c r="D403" s="33"/>
     </row>
     <row r="404" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A404" s="69"/>
-      <c r="B404" s="66"/>
-      <c r="C404" s="66"/>
+      <c r="A404" s="68"/>
+      <c r="B404" s="65"/>
+      <c r="C404" s="65"/>
       <c r="D404" s="0"/>
     </row>
     <row r="405" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16245,9 +16254,9 @@
       <c r="D406" s="33"/>
     </row>
     <row r="407" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A407" s="68"/>
-      <c r="B407" s="66"/>
-      <c r="C407" s="66"/>
+      <c r="A407" s="67"/>
+      <c r="B407" s="65"/>
+      <c r="C407" s="65"/>
       <c r="D407" s="0"/>
     </row>
     <row r="408" customFormat="false" ht="34.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16262,7 +16271,7 @@
     </row>
     <row r="409" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0"/>
-      <c r="B409" s="62" t="s">
+      <c r="B409" s="61" t="s">
         <v>238</v>
       </c>
       <c r="C409" s="0"/>
@@ -16270,17 +16279,17 @@
     </row>
     <row r="410" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0"/>
-      <c r="B410" s="62"/>
+      <c r="B410" s="61"/>
       <c r="C410" s="0"/>
       <c r="D410" s="23"/>
     </row>
     <row r="411" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A411" s="65"/>
-      <c r="B411" s="67" t="s">
+      <c r="A411" s="64"/>
+      <c r="B411" s="66" t="s">
         <v>222</v>
       </c>
-      <c r="C411" s="67"/>
-      <c r="D411" s="67"/>
+      <c r="C411" s="66"/>
+      <c r="D411" s="66"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0"/>
@@ -16299,14 +16308,14 @@
       <c r="D413" s="25"/>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A414" s="65" t="s">
+      <c r="A414" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="B414" s="67" t="s">
+      <c r="B414" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="C414" s="67"/>
-      <c r="D414" s="67"/>
+      <c r="C414" s="66"/>
+      <c r="D414" s="66"/>
     </row>
     <row r="415" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A415" s="59"/>
@@ -16315,23 +16324,23 @@
       <c r="D415" s="33"/>
     </row>
     <row r="416" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="74"/>
-      <c r="B416" s="75"/>
-      <c r="C416" s="75"/>
-      <c r="D416" s="75"/>
+      <c r="A416" s="73"/>
+      <c r="B416" s="74"/>
+      <c r="C416" s="74"/>
+      <c r="D416" s="74"/>
     </row>
     <row r="417" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A417" s="60"/>
-      <c r="B417" s="73" t="s">
+      <c r="B417" s="72" t="s">
         <v>242</v>
       </c>
-      <c r="C417" s="73"/>
-      <c r="D417" s="73"/>
+      <c r="C417" s="72"/>
+      <c r="D417" s="72"/>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="68"/>
-      <c r="B418" s="66"/>
-      <c r="C418" s="66"/>
+      <c r="A418" s="67"/>
+      <c r="B418" s="65"/>
+      <c r="C418" s="65"/>
       <c r="D418" s="0"/>
     </row>
     <row r="419" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16345,36 +16354,36 @@
       <c r="D419" s="57"/>
     </row>
     <row r="420" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="65"/>
-      <c r="B420" s="62" t="s">
+      <c r="A420" s="64"/>
+      <c r="B420" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="C420" s="66"/>
+      <c r="C420" s="65"/>
       <c r="D420" s="0"/>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="65"/>
-      <c r="B421" s="66"/>
-      <c r="C421" s="66"/>
+      <c r="A421" s="64"/>
+      <c r="B421" s="65"/>
+      <c r="C421" s="65"/>
       <c r="D421" s="0"/>
     </row>
     <row r="422" customFormat="false" ht="176.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A422" s="65"/>
-      <c r="B422" s="73" t="s">
-        <v>254</v>
-      </c>
-      <c r="C422" s="73"/>
-      <c r="D422" s="73"/>
+      <c r="A422" s="64"/>
+      <c r="B422" s="72" t="s">
+        <v>255</v>
+      </c>
+      <c r="C422" s="72"/>
+      <c r="D422" s="72"/>
     </row>
     <row r="423" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="B423" s="76" t="s">
         <v>256</v>
       </c>
-      <c r="C423" s="76"/>
-      <c r="D423" s="76"/>
+      <c r="B423" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="C423" s="75"/>
+      <c r="D423" s="75"/>
     </row>
     <row r="424" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="60" t="s">
@@ -16385,20 +16394,20 @@
       <c r="D424" s="33"/>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="69"/>
-      <c r="B425" s="66"/>
-      <c r="C425" s="66"/>
+      <c r="A425" s="68"/>
+      <c r="B425" s="65"/>
+      <c r="C425" s="65"/>
       <c r="D425" s="0"/>
     </row>
     <row r="426" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="B426" s="76" t="s">
         <v>258</v>
       </c>
-      <c r="C426" s="76"/>
-      <c r="D426" s="76"/>
+      <c r="B426" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="C426" s="75"/>
+      <c r="D426" s="75"/>
     </row>
     <row r="427" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="60" t="s">
@@ -16409,20 +16418,20 @@
       <c r="D427" s="33"/>
     </row>
     <row r="428" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="70"/>
-      <c r="B428" s="80"/>
-      <c r="C428" s="80"/>
-      <c r="D428" s="80"/>
+      <c r="A428" s="69"/>
+      <c r="B428" s="79"/>
+      <c r="C428" s="79"/>
+      <c r="D428" s="79"/>
     </row>
     <row r="429" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="B429" s="76" t="s">
         <v>260</v>
       </c>
-      <c r="C429" s="76"/>
-      <c r="D429" s="76"/>
+      <c r="B429" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="C429" s="75"/>
+      <c r="D429" s="75"/>
     </row>
     <row r="430" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="60" t="s">
@@ -16433,20 +16442,20 @@
       <c r="D430" s="33"/>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="65"/>
-      <c r="B431" s="66"/>
-      <c r="C431" s="66"/>
+      <c r="A431" s="64"/>
+      <c r="B431" s="65"/>
+      <c r="C431" s="65"/>
       <c r="D431" s="0"/>
     </row>
     <row r="432" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="B432" s="76" t="s">
         <v>262</v>
       </c>
-      <c r="C432" s="76"/>
-      <c r="D432" s="76"/>
+      <c r="B432" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="C432" s="75"/>
+      <c r="D432" s="75"/>
     </row>
     <row r="433" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="60" t="s">
@@ -16458,19 +16467,19 @@
     </row>
     <row r="434" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0"/>
-      <c r="B434" s="81"/>
-      <c r="C434" s="81"/>
-      <c r="D434" s="81"/>
+      <c r="B434" s="80"/>
+      <c r="C434" s="80"/>
+      <c r="D434" s="80"/>
     </row>
     <row r="435" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="B435" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="C435" s="76"/>
-      <c r="D435" s="76"/>
+      <c r="B435" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="C435" s="75"/>
+      <c r="D435" s="75"/>
     </row>
     <row r="436" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="60" t="s">

</xml_diff>

<commit_message>
1. Created function to add model questions to machine spreadsheet
</commit_message>
<xml_diff>
--- a/lib/machines/templates/machines.xlsx
+++ b/lib/machines/templates/machines.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="265">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machines</t>
   </si>
@@ -91,29 +91,7 @@
     <t xml:space="preserve">Internal notes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="18"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Example Machine </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <i val="true"/>
-        <sz val="18"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(note example institute is NERC but the inputs are not official)</t>
-    </r>
+    <t xml:space="preserve">Example Machine (note example institute is NERC but the inputs are not official)</t>
   </si>
   <si>
     <t xml:space="preserve">Properties of a computer/system/platform/machine which is used to run CMIP6 simulations.</t>
@@ -868,9 +846,6 @@
     <t xml:space="preserve">1.8.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">1.8.2.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOTE: Unless this entire section 1.9.2 is not applicable (due to an ‘ALL’ answer to 1.9.1), please fill out all fields in 1.9.2 except for those MIPs with NO applicable experiments; if any fields are left blank in 1.9.2 it will be taken to mean that NO experiments from the corresponding MIP were run on this machine.
 Did this machine run ALL, NO (NONE) or SOME experiments from each of the MIPs your institute is participating in (as listed separately below)? In each case, answer ALL if it is ALL, if NONE leave the field blank, and if SOME select those experiments from the (continued) enumerated list on a case-by-case basis, by entering a new row, copying &amp; pasting an existing row, and editing accordingly should you need to list multiple cases.
 Note that the listing below should cover all of the MIPs that your institute will be participating in for CMIP6 and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this.</t>
@@ -914,7 +889,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -985,15 +960,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
@@ -1116,28 +1082,6 @@
       <color rgb="FFED1C24"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFED1C24"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFED1C24"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFED1C24"/>
-      <name val="Helvetica Neue"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1267,7 +1211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="78">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1348,15 +1292,143 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1364,139 +1436,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1504,11 +1448,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1517,46 +1465,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1564,31 +1472,55 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1788,7 +1720,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12393,10 +12325,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:F1048573"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A323" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B340" activeCellId="0" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16104,14 +16036,14 @@
       <c r="B386" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="C386" s="65"/>
-      <c r="D386" s="0"/>
+      <c r="C386" s="61"/>
+      <c r="D386" s="61"/>
     </row>
     <row r="387" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A387" s="64"/>
       <c r="B387" s="61"/>
-      <c r="C387" s="65"/>
-      <c r="D387" s="0"/>
+      <c r="C387" s="61"/>
+      <c r="D387" s="61"/>
     </row>
     <row r="388" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="64"/>
@@ -16121,17 +16053,17 @@
       <c r="C388" s="72"/>
       <c r="D388" s="72"/>
     </row>
-    <row r="389" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="389" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A389" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="B389" s="75" t="s">
+      <c r="B389" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C389" s="75"/>
-      <c r="D389" s="75"/>
-    </row>
-    <row r="390" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C389" s="25"/>
+      <c r="D389" s="25"/>
+    </row>
+    <row r="390" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A390" s="60" t="s">
         <v>179</v>
       </c>
@@ -16139,408 +16071,340 @@
       <c r="C390" s="33"/>
       <c r="D390" s="33"/>
     </row>
-    <row r="391" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A391" s="68"/>
+    <row r="391" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A391" s="60"/>
       <c r="B391" s="65"/>
       <c r="C391" s="65"/>
-      <c r="D391" s="0"/>
-    </row>
-    <row r="392" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A392" s="24" t="s">
+      <c r="D391" s="65"/>
+    </row>
+    <row r="392" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A392" s="16" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="B392" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C392" s="17"/>
+      <c r="D392" s="17"/>
+    </row>
+    <row r="393" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0"/>
+      <c r="B393" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="C393" s="61"/>
+      <c r="D393" s="61"/>
+    </row>
+    <row r="394" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0"/>
+      <c r="B394" s="61"/>
+      <c r="C394" s="61"/>
+      <c r="D394" s="61"/>
+    </row>
+    <row r="395" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A395" s="64"/>
+      <c r="B395" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="C395" s="66"/>
+      <c r="D395" s="66"/>
+    </row>
+    <row r="396" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0"/>
+      <c r="B396" s="0"/>
+      <c r="C396" s="0"/>
+      <c r="D396" s="0"/>
+    </row>
+    <row r="397" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A397" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="B397" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C397" s="25"/>
+      <c r="D397" s="25"/>
+    </row>
+    <row r="398" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A398" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="B398" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C398" s="66"/>
+      <c r="D398" s="66"/>
+    </row>
+    <row r="399" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A399" s="59"/>
+      <c r="B399" s="33"/>
+      <c r="C399" s="33"/>
+      <c r="D399" s="33"/>
+    </row>
+    <row r="400" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A400" s="73"/>
+      <c r="B400" s="74"/>
+      <c r="C400" s="74"/>
+      <c r="D400" s="74"/>
+    </row>
+    <row r="401" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A401" s="60"/>
+      <c r="B401" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="C401" s="72"/>
+      <c r="D401" s="72"/>
+    </row>
+    <row r="402" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A402" s="67"/>
+      <c r="B402" s="65"/>
+      <c r="C402" s="65"/>
+      <c r="D402" s="65"/>
+    </row>
+    <row r="403" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A403" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="B403" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="C403" s="57"/>
+      <c r="D403" s="57"/>
+    </row>
+    <row r="404" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A404" s="64"/>
+      <c r="B404" s="61" t="s">
+        <v>245</v>
+      </c>
+      <c r="C404" s="61"/>
+      <c r="D404" s="61"/>
+    </row>
+    <row r="405" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A405" s="64"/>
+      <c r="B405" s="65"/>
+      <c r="C405" s="65"/>
+      <c r="D405" s="65"/>
+    </row>
+    <row r="406" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A406" s="64"/>
+      <c r="B406" s="72" t="s">
         <v>254</v>
       </c>
-      <c r="B392" s="75" t="s">
-        <v>232</v>
-      </c>
-      <c r="C392" s="75"/>
-      <c r="D392" s="75"/>
-    </row>
-    <row r="393" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A393" s="60" t="s">
+      <c r="C406" s="72"/>
+      <c r="D406" s="72"/>
+    </row>
+    <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A407" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="B407" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="C407" s="75"/>
+      <c r="D407" s="75"/>
+    </row>
+    <row r="408" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A408" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B393" s="33"/>
-      <c r="C393" s="33"/>
-      <c r="D393" s="33"/>
-    </row>
-    <row r="394" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A394" s="60"/>
-      <c r="B394" s="65"/>
-      <c r="C394" s="65"/>
-      <c r="D394" s="0"/>
-    </row>
-    <row r="395" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A395" s="76"/>
-      <c r="B395" s="77"/>
-      <c r="C395" s="77"/>
-      <c r="D395" s="78"/>
-    </row>
-    <row r="396" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A396" s="76"/>
-      <c r="B396" s="77"/>
-      <c r="C396" s="77"/>
-      <c r="D396" s="78"/>
-    </row>
-    <row r="397" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A397" s="76"/>
-      <c r="B397" s="77"/>
-      <c r="C397" s="77"/>
-      <c r="D397" s="78"/>
-    </row>
-    <row r="398" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A398" s="76"/>
-      <c r="B398" s="77"/>
-      <c r="C398" s="77"/>
-      <c r="D398" s="78"/>
-    </row>
-    <row r="399" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A399" s="76"/>
-      <c r="B399" s="77"/>
-      <c r="C399" s="77"/>
-      <c r="D399" s="78"/>
-    </row>
-    <row r="400" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A400" s="76"/>
-      <c r="B400" s="77"/>
-      <c r="C400" s="77"/>
-      <c r="D400" s="78"/>
-    </row>
-    <row r="401" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A401" s="60"/>
-      <c r="B401" s="65"/>
-      <c r="C401" s="65"/>
-      <c r="D401" s="0"/>
-    </row>
-    <row r="402" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A402" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="B402" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="C402" s="25"/>
-      <c r="D402" s="25"/>
-    </row>
-    <row r="403" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A403" s="60" t="s">
+      <c r="B408" s="33"/>
+      <c r="C408" s="33"/>
+      <c r="D408" s="33"/>
+    </row>
+    <row r="409" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A409" s="68"/>
+      <c r="B409" s="65"/>
+      <c r="C409" s="65"/>
+      <c r="D409" s="65"/>
+    </row>
+    <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A410" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B410" s="75" t="s">
+        <v>258</v>
+      </c>
+      <c r="C410" s="75"/>
+      <c r="D410" s="75"/>
+    </row>
+    <row r="411" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A411" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B403" s="33"/>
-      <c r="C403" s="33"/>
-      <c r="D403" s="33"/>
-    </row>
-    <row r="404" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A404" s="68"/>
-      <c r="B404" s="65"/>
-      <c r="C404" s="65"/>
-      <c r="D404" s="0"/>
-    </row>
-    <row r="405" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A405" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="B405" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C405" s="25"/>
-      <c r="D405" s="25"/>
-    </row>
-    <row r="406" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A406" s="60" t="s">
+      <c r="B411" s="33"/>
+      <c r="C411" s="33"/>
+      <c r="D411" s="33"/>
+    </row>
+    <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A412" s="69"/>
+      <c r="B412" s="76"/>
+      <c r="C412" s="76"/>
+      <c r="D412" s="76"/>
+    </row>
+    <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A413" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="B413" s="75" t="s">
+        <v>260</v>
+      </c>
+      <c r="C413" s="75"/>
+      <c r="D413" s="75"/>
+    </row>
+    <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A414" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B406" s="33"/>
-      <c r="C406" s="33"/>
-      <c r="D406" s="33"/>
-    </row>
-    <row r="407" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A407" s="67"/>
-      <c r="B407" s="65"/>
-      <c r="C407" s="65"/>
-      <c r="D407" s="0"/>
-    </row>
-    <row r="408" customFormat="false" ht="34.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A408" s="16" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="B408" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="C408" s="17"/>
-      <c r="D408" s="17"/>
-    </row>
-    <row r="409" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="0"/>
-      <c r="B409" s="61" t="s">
-        <v>238</v>
-      </c>
-      <c r="C409" s="0"/>
-      <c r="D409" s="23"/>
-    </row>
-    <row r="410" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="0"/>
-      <c r="B410" s="61"/>
-      <c r="C410" s="0"/>
-      <c r="D410" s="23"/>
-    </row>
-    <row r="411" customFormat="false" ht="28.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A411" s="64"/>
-      <c r="B411" s="66" t="s">
-        <v>222</v>
-      </c>
-      <c r="C411" s="66"/>
-      <c r="D411" s="66"/>
-    </row>
-    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="0"/>
-      <c r="B412" s="0"/>
-      <c r="C412" s="0"/>
-      <c r="D412" s="0"/>
-    </row>
-    <row r="413" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="B413" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="C413" s="25"/>
-      <c r="D413" s="25"/>
-    </row>
-    <row r="414" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A414" s="64" t="s">
+      <c r="B414" s="33"/>
+      <c r="C414" s="33"/>
+      <c r="D414" s="33"/>
+    </row>
+    <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A415" s="64"/>
+      <c r="B415" s="65"/>
+      <c r="C415" s="65"/>
+      <c r="D415" s="65"/>
+    </row>
+    <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A416" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B416" s="75" t="s">
+        <v>262</v>
+      </c>
+      <c r="C416" s="75"/>
+      <c r="D416" s="75"/>
+    </row>
+    <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A417" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B414" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="C414" s="66"/>
-      <c r="D414" s="66"/>
-    </row>
-    <row r="415" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A415" s="59"/>
-      <c r="B415" s="33"/>
-      <c r="C415" s="33"/>
-      <c r="D415" s="33"/>
-    </row>
-    <row r="416" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="73"/>
-      <c r="B416" s="74"/>
-      <c r="C416" s="74"/>
-      <c r="D416" s="74"/>
-    </row>
-    <row r="417" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A417" s="60"/>
-      <c r="B417" s="72" t="s">
-        <v>242</v>
-      </c>
-      <c r="C417" s="72"/>
-      <c r="D417" s="72"/>
-    </row>
-    <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="67"/>
-      <c r="B418" s="65"/>
-      <c r="C418" s="65"/>
-      <c r="D418" s="0"/>
-    </row>
-    <row r="419" customFormat="false" ht="33.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A419" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="B419" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="C419" s="57"/>
-      <c r="D419" s="57"/>
-    </row>
-    <row r="420" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="64"/>
-      <c r="B420" s="61" t="s">
-        <v>245</v>
-      </c>
-      <c r="C420" s="65"/>
-      <c r="D420" s="0"/>
-    </row>
-    <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="64"/>
-      <c r="B421" s="65"/>
-      <c r="C421" s="65"/>
-      <c r="D421" s="0"/>
-    </row>
-    <row r="422" customFormat="false" ht="176.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A422" s="64"/>
-      <c r="B422" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="C422" s="72"/>
-      <c r="D422" s="72"/>
-    </row>
-    <row r="423" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="B423" s="75" t="s">
-        <v>257</v>
-      </c>
-      <c r="C423" s="75"/>
-      <c r="D423" s="75"/>
-    </row>
-    <row r="424" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="60" t="s">
+      <c r="B417" s="33"/>
+      <c r="C417" s="33"/>
+      <c r="D417" s="33"/>
+    </row>
+    <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0"/>
+      <c r="B418" s="77"/>
+      <c r="C418" s="77"/>
+      <c r="D418" s="77"/>
+    </row>
+    <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A419" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="B419" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="C419" s="75"/>
+      <c r="D419" s="75"/>
+    </row>
+    <row r="420" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A420" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B424" s="33"/>
-      <c r="C424" s="33"/>
-      <c r="D424" s="33"/>
-    </row>
-    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="68"/>
-      <c r="B425" s="65"/>
-      <c r="C425" s="65"/>
-      <c r="D425" s="0"/>
-    </row>
-    <row r="426" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="B426" s="75" t="s">
-        <v>259</v>
-      </c>
-      <c r="C426" s="75"/>
-      <c r="D426" s="75"/>
-    </row>
-    <row r="427" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B427" s="33"/>
-      <c r="C427" s="33"/>
-      <c r="D427" s="33"/>
-    </row>
-    <row r="428" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="69"/>
-      <c r="B428" s="79"/>
-      <c r="C428" s="79"/>
-      <c r="D428" s="79"/>
-    </row>
-    <row r="429" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="B429" s="75" t="s">
-        <v>261</v>
-      </c>
-      <c r="C429" s="75"/>
-      <c r="D429" s="75"/>
-    </row>
-    <row r="430" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B430" s="33"/>
-      <c r="C430" s="33"/>
-      <c r="D430" s="33"/>
-    </row>
-    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="64"/>
-      <c r="B431" s="65"/>
-      <c r="C431" s="65"/>
-      <c r="D431" s="0"/>
-    </row>
-    <row r="432" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="B432" s="75" t="s">
-        <v>263</v>
-      </c>
-      <c r="C432" s="75"/>
-      <c r="D432" s="75"/>
-    </row>
-    <row r="433" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B433" s="33"/>
-      <c r="C433" s="33"/>
-      <c r="D433" s="33"/>
-    </row>
-    <row r="434" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="0"/>
-      <c r="B434" s="80"/>
-      <c r="C434" s="80"/>
-      <c r="D434" s="80"/>
-    </row>
-    <row r="435" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="B435" s="75" t="s">
-        <v>265</v>
-      </c>
-      <c r="C435" s="75"/>
-      <c r="D435" s="75"/>
-    </row>
-    <row r="436" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B436" s="33"/>
-      <c r="C436" s="33"/>
-      <c r="D436" s="33"/>
-    </row>
-    <row r="437" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B420" s="33"/>
+      <c r="C420" s="33"/>
+      <c r="D420" s="33"/>
+    </row>
+    <row r="421" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16592,13 +16456,11 @@
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="197">
+  <mergeCells count="205">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B9:D9"/>
@@ -16768,57 +16630,61 @@
     <mergeCell ref="B381:D381"/>
     <mergeCell ref="B382:D382"/>
     <mergeCell ref="B383:D383"/>
+    <mergeCell ref="B385:D385"/>
+    <mergeCell ref="B386:D386"/>
+    <mergeCell ref="B387:D387"/>
     <mergeCell ref="B388:D388"/>
     <mergeCell ref="B389:D389"/>
     <mergeCell ref="B390:D390"/>
+    <mergeCell ref="B391:D391"/>
     <mergeCell ref="B392:D392"/>
     <mergeCell ref="B393:D393"/>
+    <mergeCell ref="B394:D394"/>
+    <mergeCell ref="B395:D395"/>
+    <mergeCell ref="B396:D396"/>
+    <mergeCell ref="B397:D397"/>
+    <mergeCell ref="B398:D398"/>
+    <mergeCell ref="B399:D399"/>
+    <mergeCell ref="B400:D400"/>
+    <mergeCell ref="B401:D401"/>
     <mergeCell ref="B402:D402"/>
     <mergeCell ref="B403:D403"/>
+    <mergeCell ref="B404:D404"/>
     <mergeCell ref="B405:D405"/>
     <mergeCell ref="B406:D406"/>
+    <mergeCell ref="B407:D407"/>
     <mergeCell ref="B408:D408"/>
+    <mergeCell ref="B409:D409"/>
+    <mergeCell ref="B410:D410"/>
     <mergeCell ref="B411:D411"/>
+    <mergeCell ref="B412:D412"/>
     <mergeCell ref="B413:D413"/>
     <mergeCell ref="B414:D414"/>
     <mergeCell ref="B415:D415"/>
     <mergeCell ref="B416:D416"/>
     <mergeCell ref="B417:D417"/>
-    <mergeCell ref="B422:D422"/>
-    <mergeCell ref="B423:D423"/>
-    <mergeCell ref="B424:D424"/>
-    <mergeCell ref="B426:D426"/>
-    <mergeCell ref="B427:D427"/>
-    <mergeCell ref="B428:D428"/>
-    <mergeCell ref="B429:D429"/>
-    <mergeCell ref="B430:D430"/>
-    <mergeCell ref="B432:D432"/>
-    <mergeCell ref="B433:D433"/>
-    <mergeCell ref="B435:D435"/>
-    <mergeCell ref="B436:D436"/>
+    <mergeCell ref="B418:D418"/>
+    <mergeCell ref="B419:D419"/>
+    <mergeCell ref="B420:D420"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B303 B334" type="list">
       <formula1>"Lustre: Lustre parallel file system.,GPFS: IBM GPFS (also known as IBM Spectral Scale.,isilon: The EMC scaleout NAS solution.,NFS: Generic Network File System.,S3: Object file system exposing the AWS S3 interface.,PanFS: Panasas Parallel File system.,Othe"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B381 B415" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B381 B399" type="list">
       <formula1>"ALL,SOME"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B424 B427 B430 B433 B436" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B408 B411 B414 B417 B420" type="list">
       <formula1>"ALL,EXPERIMENT 1 INSTITUTE INVOLVED IN FROM THIS MIP,EXPERIMENT 2 [AS ABOVE],...,...,...,EXPERIMENT  N [FINAL ONE POSSIBLE FOR GIVEN INSTITUTE AND MIP]"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B390 B393 B403 B406" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B390" type="list">
       <formula1>"YES,NO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B388" r:id="rId1" display="Did this machine run each of the following models? For each model, if it was run on this machine select YES, else select NO.&#10;&#10;Note that the listing below should cover all of the models that your institute will be running for CMIP6 (on one of your machines, but perhaps not this one) and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this."/>
-    <hyperlink ref="B422" r:id="rId2" display="NOTE: Unless this entire section 1.9.2 is not applicable (due to an ‘ALL’ answer to 1.9.1), please fill out all fields in 1.9.2 except for those MIPs with NO applicable experiments; if any fields are left blank in 1.9.2 it will be taken to mean that NO experiments from the corresponding MIP were run on this machine.&#10;&#10;Did this machine run ALL, NO (NONE) or SOME experiments from each of the MIPs your institute is participating in (as listed separately below)? In each case, answer ALL if it is ALL, if NONE leave the field blank, and if SOME select those experiments from the (continued) enumerated list on a case-by-case basis, by entering a new row, copying &amp; pasting an existing row, and editing accordingly should you need to list multiple cases.&#10;&#10;Note that the listing below should cover all of the MIPs that your institute will be participating in for CMIP6 and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this."/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1. Added function to make machine spreadsheet experiment questions
</commit_message>
<xml_diff>
--- a/lib/machines/templates/machines.xlsx
+++ b/lib/machines/templates/machines.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="258">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machines</t>
   </si>
@@ -846,39 +846,41 @@
     <t xml:space="preserve">1.8.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTE: Unless this entire section 1.9.2 is not applicable (due to an ‘ALL’ answer to 1.9.1), please fill out all fields in 1.9.2 except for those MIPs with NO applicable experiments; if any fields are left blank in 1.9.2 it will be taken to mean that NO experiments from the corresponding MIP were run on this machine.
-Did this machine run ALL, NO (NONE) or SOME experiments from each of the MIPs your institute is participating in (as listed separately below)? In each case, answer ALL if it is ALL, if NONE leave the field blank, and if SOME select those experiments from the (continued) enumerated list on a case-by-case basis, by entering a new row, copying &amp; pasting an existing row, and editing accordingly should you need to list multiple cases.
-Note that the listing below should cover all of the MIPs that your institute will be participating in for CMIP6 and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this.</t>
+    <t xml:space="preserve">Has this machine run all applicable experiments from ALL of the MIPs your institute is participating in, or just SOME of them?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: Unless this entire section 1.9.2 is not applicable (due to an ‘ALL’ answer to 1.9.1), please fill out all fields in 1.9.2 except for those MIPs with NO applicable experiments; if any fields are left blank in 1.9.2 it will be taken to mean that NO experiments from the corresponding MIP were run on this machine.
+Did this machine run ALL, NO (NONE) or SOME experiments from each of the MIPs that your institute is participating in (as listed separately below)? In each case, answer ALL if it is ALL, NONE if it is NO experiments, and if SOME select those experiments from the (continued) enumerated list on a case-by-case basis, by entering a new (input box) row, copying &amp; pasting an existing row, and editing accordingly should you need to list multiple cases.
+Note that in cases where there is only one experiment applicable, the answer will be pre-populated with that one experiment selected, so you do not need to do anything.
+Note that the listing below should cover all of the MIPs that your institute will be participating in for CMIP6 and if that is not the case, please contact the ES-DOC team via support@es-doc.org so we can check this.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">1.9.2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">AerChemMIP: Aerosols and Chemistry MIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.9.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4MIP: Coupled Climate Carbon Cycle MIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.9.2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDRMIP: The Carbon Dioxide Removal MIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.9.2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CFMIP: Cloud Feedback MIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.9.2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAMIP: Detection and Attribution MIP</t>
+    <t xml:space="preserve">&lt;MIP goes here&gt;</t>
   </si>
 </sst>
 </file>
@@ -1078,18 +1080,16 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFED1C24"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFED1C24"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1211,7 +1211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1512,16 +1512,24 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1537,7 +1545,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFED1C24"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1587,7 +1595,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF5C2D91"/>
       <rgbColor rgb="FF333333"/>
@@ -12325,10 +12333,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F1048573"/>
+  <dimension ref="A1:F410"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A323" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B340" activeCellId="0" sqref="B340"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A394" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G407" activeCellId="0" sqref="G407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16025,25 +16033,25 @@
       <c r="A385" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="B385" s="57" t="s">
+      <c r="B385" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="C385" s="57"/>
-      <c r="D385" s="57"/>
+      <c r="C385" s="75"/>
+      <c r="D385" s="75"/>
     </row>
     <row r="386" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A386" s="64"/>
-      <c r="B386" s="61" t="s">
+      <c r="B386" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="C386" s="61"/>
-      <c r="D386" s="61"/>
+      <c r="C386" s="76"/>
+      <c r="D386" s="76"/>
     </row>
     <row r="387" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A387" s="64"/>
-      <c r="B387" s="61"/>
-      <c r="C387" s="61"/>
-      <c r="D387" s="61"/>
+      <c r="B387" s="76"/>
+      <c r="C387" s="76"/>
+      <c r="D387" s="76"/>
     </row>
     <row r="388" customFormat="false" ht="97.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="64"/>
@@ -16073,9 +16081,9 @@
     </row>
     <row r="391" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A391" s="60"/>
-      <c r="B391" s="65"/>
-      <c r="C391" s="65"/>
-      <c r="D391" s="65"/>
+      <c r="B391" s="77"/>
+      <c r="C391" s="77"/>
+      <c r="D391" s="77"/>
     </row>
     <row r="392" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A392" s="16" t="n">
@@ -16089,17 +16097,17 @@
     </row>
     <row r="393" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A393" s="0"/>
-      <c r="B393" s="61" t="s">
+      <c r="B393" s="76" t="s">
         <v>238</v>
       </c>
-      <c r="C393" s="61"/>
-      <c r="D393" s="61"/>
+      <c r="C393" s="76"/>
+      <c r="D393" s="76"/>
     </row>
     <row r="394" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A394" s="0"/>
-      <c r="B394" s="61"/>
-      <c r="C394" s="61"/>
-      <c r="D394" s="61"/>
+      <c r="B394" s="76"/>
+      <c r="C394" s="76"/>
+      <c r="D394" s="76"/>
     </row>
     <row r="395" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A395" s="64"/>
@@ -16111,9 +16119,9 @@
     </row>
     <row r="396" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A396" s="0"/>
-      <c r="B396" s="0"/>
-      <c r="C396" s="0"/>
-      <c r="D396" s="0"/>
+      <c r="B396" s="78"/>
+      <c r="C396" s="78"/>
+      <c r="D396" s="78"/>
     </row>
     <row r="397" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A397" s="24" t="s">
@@ -16130,7 +16138,7 @@
         <v>179</v>
       </c>
       <c r="B398" s="66" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="C398" s="66"/>
       <c r="D398" s="66"/>
@@ -16157,156 +16165,77 @@
     </row>
     <row r="402" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A402" s="67"/>
-      <c r="B402" s="65"/>
-      <c r="C402" s="65"/>
-      <c r="D402" s="65"/>
+      <c r="B402" s="77"/>
+      <c r="C402" s="77"/>
+      <c r="D402" s="77"/>
     </row>
     <row r="403" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A403" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="B403" s="57" t="s">
+      <c r="B403" s="75" t="s">
         <v>244</v>
       </c>
-      <c r="C403" s="57"/>
-      <c r="D403" s="57"/>
+      <c r="C403" s="75"/>
+      <c r="D403" s="75"/>
     </row>
     <row r="404" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A404" s="64"/>
-      <c r="B404" s="61" t="s">
+      <c r="B404" s="76" t="s">
         <v>245</v>
       </c>
-      <c r="C404" s="61"/>
-      <c r="D404" s="61"/>
+      <c r="C404" s="76"/>
+      <c r="D404" s="76"/>
     </row>
     <row r="405" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A405" s="64"/>
-      <c r="B405" s="65"/>
-      <c r="C405" s="65"/>
-      <c r="D405" s="65"/>
+      <c r="B405" s="77"/>
+      <c r="C405" s="77"/>
+      <c r="D405" s="77"/>
     </row>
     <row r="406" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A406" s="64"/>
-      <c r="B406" s="72" t="s">
-        <v>254</v>
-      </c>
-      <c r="C406" s="72"/>
-      <c r="D406" s="72"/>
+      <c r="B406" s="79" t="s">
+        <v>255</v>
+      </c>
+      <c r="C406" s="79"/>
+      <c r="D406" s="79"/>
     </row>
     <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A407" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="B407" s="75" t="s">
+      <c r="A407" s="64"/>
+      <c r="B407" s="72"/>
+      <c r="C407" s="72"/>
+      <c r="D407" s="72"/>
+    </row>
+    <row r="408" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A408" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="C407" s="75"/>
-      <c r="D407" s="75"/>
-    </row>
-    <row r="408" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A408" s="60" t="s">
+      <c r="B408" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C408" s="25"/>
+      <c r="D408" s="25"/>
+    </row>
+    <row r="409" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A409" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="B408" s="33"/>
-      <c r="C408" s="33"/>
-      <c r="D408" s="33"/>
-    </row>
-    <row r="409" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A409" s="68"/>
-      <c r="B409" s="65"/>
-      <c r="C409" s="65"/>
-      <c r="D409" s="65"/>
-    </row>
-    <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A410" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="B410" s="75" t="s">
-        <v>258</v>
-      </c>
-      <c r="C410" s="75"/>
-      <c r="D410" s="75"/>
-    </row>
-    <row r="411" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A411" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B411" s="33"/>
-      <c r="C411" s="33"/>
-      <c r="D411" s="33"/>
-    </row>
-    <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A412" s="69"/>
-      <c r="B412" s="76"/>
-      <c r="C412" s="76"/>
-      <c r="D412" s="76"/>
-    </row>
-    <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A413" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="B413" s="75" t="s">
-        <v>260</v>
-      </c>
-      <c r="C413" s="75"/>
-      <c r="D413" s="75"/>
-    </row>
-    <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A414" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B414" s="33"/>
-      <c r="C414" s="33"/>
-      <c r="D414" s="33"/>
-    </row>
-    <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A415" s="64"/>
-      <c r="B415" s="65"/>
-      <c r="C415" s="65"/>
-      <c r="D415" s="65"/>
-    </row>
-    <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A416" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="B416" s="75" t="s">
-        <v>262</v>
-      </c>
-      <c r="C416" s="75"/>
-      <c r="D416" s="75"/>
-    </row>
-    <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A417" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B417" s="33"/>
-      <c r="C417" s="33"/>
-      <c r="D417" s="33"/>
-    </row>
-    <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A418" s="0"/>
-      <c r="B418" s="77"/>
-      <c r="C418" s="77"/>
-      <c r="D418" s="77"/>
-    </row>
-    <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A419" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="B419" s="75" t="s">
-        <v>264</v>
-      </c>
-      <c r="C419" s="75"/>
-      <c r="D419" s="75"/>
-    </row>
-    <row r="420" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A420" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="B420" s="33"/>
-      <c r="C420" s="33"/>
-      <c r="D420" s="33"/>
-    </row>
+      <c r="B409" s="33"/>
+      <c r="C409" s="33"/>
+      <c r="D409" s="33"/>
+    </row>
+    <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="421" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="422" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="423" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -16389,78 +16318,9 @@
     <row r="500" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="501" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="502" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="205">
+  <mergeCells count="193">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B9:D9"/>
@@ -16652,32 +16512,16 @@
     <mergeCell ref="B404:D404"/>
     <mergeCell ref="B405:D405"/>
     <mergeCell ref="B406:D406"/>
-    <mergeCell ref="B407:D407"/>
     <mergeCell ref="B408:D408"/>
     <mergeCell ref="B409:D409"/>
-    <mergeCell ref="B410:D410"/>
-    <mergeCell ref="B411:D411"/>
-    <mergeCell ref="B412:D412"/>
-    <mergeCell ref="B413:D413"/>
-    <mergeCell ref="B414:D414"/>
-    <mergeCell ref="B415:D415"/>
-    <mergeCell ref="B416:D416"/>
-    <mergeCell ref="B417:D417"/>
-    <mergeCell ref="B418:D418"/>
-    <mergeCell ref="B419:D419"/>
-    <mergeCell ref="B420:D420"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B303 B334" type="list">
       <formula1>"Lustre: Lustre parallel file system.,GPFS: IBM GPFS (also known as IBM Spectral Scale.,isilon: The EMC scaleout NAS solution.,NFS: Generic Network File System.,S3: Object file system exposing the AWS S3 interface.,PanFS: Panasas Parallel File system.,Othe"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B381 B399" type="list">
       <formula1>"ALL,SOME"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B408 B411 B414 B417 B420" type="list">
-      <formula1>"ALL,EXPERIMENT 1 INSTITUTE INVOLVED IN FROM THIS MIP,EXPERIMENT 2 [AS ABOVE],...,...,...,EXPERIMENT  N [FINAL ONE POSSIBLE FOR GIVEN INSTITUTE AND MIP]"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B390" type="list">

</xml_diff>